<commit_message>
Adicionando idh em .csv
</commit_message>
<xml_diff>
--- a/data/idh_2021.xlsx
+++ b/data/idh_2021.xlsx
@@ -1,21 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/865a58d3a781240e/Estudo/maua/ciencia_dados/enem_analytics/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_9D3185EEF1D7E755E69D8BF3B613D0A8ADC68498" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86707853-5E2C-43B6-BB4F-BCCFF204A6DA}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Territorialidades</t>
   </si>
@@ -105,37 +123,20 @@
   </si>
   <si>
     <t>Tocantins</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Elaboração: Atlas do Desenvolvimento Humano no Brasil. Pnud Brasil, Ipea e FJP, 2022.</t>
-  </si>
-  <si>
-    <t>Fontes: dados do IBGE e de registros administrativos, conforme especificados nos metadados disponíveis disponíveis em: http://atlasbrasil.org.br/acervo/biblioteca.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -150,24 +151,34 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -457,23 +468,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:ZZ32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:ZZ29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1:ZZ1"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="193" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="193" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:702">
+    <row r="1" spans="1:702" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1181,15 +1189,15 @@
       <c r="ZY1" s="1"/>
       <c r="ZZ1" s="1"/>
     </row>
-    <row r="2" spans="1:702">
+    <row r="2" spans="1:702" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.766</v>
-      </c>
-    </row>
-    <row r="3" spans="1:702">
+        <v>0.76600000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:702" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1197,23 +1205,23 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="4" spans="1:702">
+    <row r="4" spans="1:702" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.684</v>
-      </c>
-    </row>
-    <row r="5" spans="1:702">
+        <v>0.68400000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:702" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.688</v>
-      </c>
-    </row>
-    <row r="6" spans="1:702">
+        <v>0.68799999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:702" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1221,95 +1229,95 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:702">
+    <row r="7" spans="1:702" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.691</v>
-      </c>
-    </row>
-    <row r="8" spans="1:702">
+        <v>0.69099999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:702" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.734</v>
-      </c>
-    </row>
-    <row r="9" spans="1:702">
+        <v>0.73399999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:702" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.814</v>
-      </c>
-    </row>
-    <row r="10" spans="1:702">
+        <v>0.81399999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:702" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.771</v>
-      </c>
-    </row>
-    <row r="11" spans="1:702">
+        <v>0.77100000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:702" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.737</v>
-      </c>
-    </row>
-    <row r="12" spans="1:702">
+        <v>0.73699999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:702" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.676</v>
-      </c>
-    </row>
-    <row r="13" spans="1:702">
+        <v>0.67600000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:702" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.742</v>
-      </c>
-    </row>
-    <row r="14" spans="1:702">
+        <v>0.74199999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:702" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0.736</v>
-      </c>
-    </row>
-    <row r="15" spans="1:702">
+        <v>0.73599999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:702" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0.774</v>
-      </c>
-    </row>
-    <row r="16" spans="1:702">
+        <v>0.77400000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:702" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0.698</v>
-      </c>
-    </row>
-    <row r="17" spans="1:702">
+        <v>0.69799999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0.769</v>
-      </c>
-    </row>
-    <row r="18" spans="1:702">
+        <v>0.76900000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1317,15 +1325,15 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="19" spans="1:702">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0.719</v>
-      </c>
-    </row>
-    <row r="20" spans="1:702">
+        <v>0.71899999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1333,31 +1341,31 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="21" spans="1:702">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21">
-        <v>0.762</v>
-      </c>
-    </row>
-    <row r="22" spans="1:702">
+        <v>0.76200000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
-        <v>0.728</v>
-      </c>
-    </row>
-    <row r="23" spans="1:702">
+        <v>0.72799999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
-        <v>0.771</v>
-      </c>
-    </row>
-    <row r="24" spans="1:702">
+        <v>0.77100000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1365,77 +1373,48 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="25" spans="1:702">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25">
-        <v>0.699</v>
-      </c>
-    </row>
-    <row r="26" spans="1:702">
+        <v>0.69899999999999995</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26">
-        <v>0.792</v>
-      </c>
-    </row>
-    <row r="27" spans="1:702">
+        <v>0.79200000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27">
-        <v>0.806</v>
-      </c>
-    </row>
-    <row r="28" spans="1:702">
+        <v>0.80600000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28">
-        <v>0.702</v>
-      </c>
-    </row>
-    <row r="29" spans="1:702">
+        <v>0.70199999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29">
-        <v>0.731</v>
-      </c>
-    </row>
-    <row r="30" spans="1:702">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:702">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:702">
-      <c r="A32" t="s">
-        <v>32</v>
+        <v>0.73099999999999998</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>